<commit_message>
update get_tweets without tweepy
</commit_message>
<xml_diff>
--- a/ressources/data/data_history.xlsx
+++ b/ressources/data/data_history.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="106">
   <si>
     <t xml:space="preserve">date_last_update</t>
   </si>
@@ -52,10 +52,10 @@
     <t xml:space="preserve">afpfr</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-05-16 21:50:00</t>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010-05-16 21:50:00</t>
   </si>
   <si>
     <t xml:space="preserve">938522598585131008</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">AuroreLalucq</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 15:54:35</t>
+    <t xml:space="preserve">2010-05-16 21:50:01</t>
   </si>
   <si>
     <t xml:space="preserve">133663801</t>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">BFMTV</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 23:29:14</t>
+    <t xml:space="preserve">2010-05-16 21:50:02</t>
   </si>
   <si>
     <t xml:space="preserve">472852289</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">Brevesdepresse</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 20:37:47</t>
+    <t xml:space="preserve">2010-05-16 21:50:03</t>
   </si>
   <si>
     <t xml:space="preserve">765849247262633984</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">brutofficiel</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 19:54:04</t>
+    <t xml:space="preserve">2010-05-16 21:50:04</t>
   </si>
   <si>
     <t xml:space="preserve">971820228</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">CerfiaFR</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 17:45:15</t>
+    <t xml:space="preserve">2010-05-16 21:50:05</t>
   </si>
   <si>
     <t xml:space="preserve">1976143068</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">EmmanuelMacron</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 21:03:41</t>
+    <t xml:space="preserve">2010-05-16 21:50:06</t>
   </si>
   <si>
     <t xml:space="preserve">53029114</t>
@@ -118,7 +118,7 @@
     <t xml:space="preserve">humanite_fr</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 18:00:02</t>
+    <t xml:space="preserve">2010-05-16 21:50:07</t>
   </si>
   <si>
     <t xml:space="preserve">1233151236154761217</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">L_ThinkTank</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 20:20:32</t>
+    <t xml:space="preserve">2010-05-16 21:50:08</t>
   </si>
   <si>
     <t xml:space="preserve">26110930</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">LCI</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 21:45:45</t>
+    <t xml:space="preserve">2010-05-16 21:50:09</t>
   </si>
   <si>
     <t xml:space="preserve">24744541</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">lemondefr</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 23:29:38</t>
+    <t xml:space="preserve">2010-05-16 21:50:10</t>
   </si>
   <si>
     <t xml:space="preserve">92564226</t>
@@ -154,7 +154,7 @@
     <t xml:space="preserve">LesEchos</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 19:38:26</t>
+    <t xml:space="preserve">2010-05-16 21:50:11</t>
   </si>
   <si>
     <t xml:space="preserve">68440549</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">libe</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 23:20:59</t>
+    <t xml:space="preserve">2010-05-16 21:50:12</t>
   </si>
   <si>
     <t xml:space="preserve">2729039440</t>
@@ -172,7 +172,7 @@
     <t xml:space="preserve">nico_dufrene</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-05 09:20:39</t>
+    <t xml:space="preserve">2010-05-16 21:50:13</t>
   </si>
   <si>
     <t xml:space="preserve">959531564341317632</t>
@@ -181,7 +181,7 @@
     <t xml:space="preserve">AlertesInfos</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-05-16 18:59:30</t>
+    <t xml:space="preserve">2010-05-16 21:50:14</t>
   </si>
   <si>
     <t xml:space="preserve">2023-05-17 00:00:00</t>
@@ -193,100 +193,151 @@
     <t xml:space="preserve">i24NEWS_FR</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:15</t>
+  </si>
+  <si>
     <t xml:space="preserve">25048816</t>
   </si>
   <si>
     <t xml:space="preserve">France24_fr</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:16</t>
+  </si>
+  <si>
     <t xml:space="preserve">32861321</t>
   </si>
   <si>
     <t xml:space="preserve">RFI</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:17</t>
+  </si>
+  <si>
     <t xml:space="preserve">23424509</t>
   </si>
   <si>
     <t xml:space="preserve">TV5MONDE</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:18</t>
+  </si>
+  <si>
     <t xml:space="preserve">8460572</t>
   </si>
   <si>
     <t xml:space="preserve">LePoint</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:19</t>
+  </si>
+  <si>
     <t xml:space="preserve">364513528</t>
   </si>
   <si>
     <t xml:space="preserve">LeHuffPost</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:20</t>
+  </si>
+  <si>
     <t xml:space="preserve">743432061088899073</t>
   </si>
   <si>
     <t xml:space="preserve">Qofficiel</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:21</t>
+  </si>
+  <si>
     <t xml:space="preserve">34867057</t>
   </si>
   <si>
     <t xml:space="preserve">franceinter</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:22</t>
+  </si>
+  <si>
     <t xml:space="preserve">34570323</t>
   </si>
   <si>
     <t xml:space="preserve">Europe1</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:23</t>
+  </si>
+  <si>
     <t xml:space="preserve">38142665</t>
   </si>
   <si>
     <t xml:space="preserve">le_Parisien</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:24</t>
+  </si>
+  <si>
     <t xml:space="preserve">8350912</t>
   </si>
   <si>
     <t xml:space="preserve">Le_Figaro</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:25</t>
+  </si>
+  <si>
     <t xml:space="preserve">19976004</t>
   </si>
   <si>
     <t xml:space="preserve">Mediapart</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:26</t>
+  </si>
+  <si>
     <t xml:space="preserve">13353862</t>
   </si>
   <si>
     <t xml:space="preserve">LEXPRESS</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:27</t>
+  </si>
+  <si>
     <t xml:space="preserve">596420812</t>
   </si>
   <si>
     <t xml:space="preserve">canardenchaine</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:28</t>
+  </si>
+  <si>
     <t xml:space="preserve">21313364</t>
   </si>
   <si>
     <t xml:space="preserve">lobs</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:29</t>
+  </si>
+  <si>
     <t xml:space="preserve">34294667</t>
   </si>
   <si>
     <t xml:space="preserve">RTLFrance</t>
   </si>
   <si>
+    <t xml:space="preserve">2010-05-16 21:50:30</t>
+  </si>
+  <si>
     <t xml:space="preserve">2649991</t>
   </si>
   <si>
     <t xml:space="preserve">20Minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2010-05-16 21:50:31</t>
   </si>
 </sst>
 </file>
@@ -413,11 +464,11 @@
   </sheetPr>
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.74"/>
@@ -764,7 +815,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,16 +826,16 @@
         <v>7</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,16 +846,16 @@
         <v>7</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -815,16 +866,16 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -835,16 +886,16 @@
         <v>7</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,16 +906,16 @@
         <v>7</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -875,16 +926,16 @@
         <v>7</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>54</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -895,16 +946,16 @@
         <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -915,16 +966,16 @@
         <v>7</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -935,16 +986,16 @@
         <v>7</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -955,16 +1006,16 @@
         <v>7</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,16 +1026,16 @@
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>54</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -995,16 +1046,16 @@
         <v>7</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1015,16 +1066,16 @@
         <v>7</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>54</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1035,16 +1086,16 @@
         <v>7</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1055,16 +1106,16 @@
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,16 +1126,16 @@
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>